<commit_message>
changed canbusids made Regler_Controller easier to configure
</commit_message>
<xml_diff>
--- a/CAN_BUS_IDs.xlsx
+++ b/CAN_BUS_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\philipp\git\Diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E14D7F-8EE3-4B98-A2E2-6C2D695403C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A671276F-A626-4FAC-A25B-8979AB92405B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59229394-A23F-41AD-8842-C58804BC4CA3}"/>
+    <workbookView xWindow="4128" yWindow="348" windowWidth="9204" windowHeight="9060" xr2:uid="{59229394-A23F-41AD-8842-C58804BC4CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Info</t>
   </si>
   <si>
-    <t>CAN_ID_CONTROL_LOWER_MOTOR</t>
-  </si>
-  <si>
     <t>CAN_ID_INFOS_LOWER_CONTROLLER</t>
   </si>
   <si>
@@ -57,12 +54,6 @@
     <t>0xC1</t>
   </si>
   <si>
-    <t>0xC2</t>
-  </si>
-  <si>
-    <t>CAN_ID_CONTROL_BACK_MOTOR</t>
-  </si>
-  <si>
     <t>CAN_ID_INFOS_BACK_CONTROLLER</t>
   </si>
   <si>
@@ -85,6 +76,9 @@
   </si>
   <si>
     <t>Kontrolliert die für die Lenkung zuständigen Servos</t>
+  </si>
+  <si>
+    <t>CAN_ID_CONTROL_MOTORS_SERVOS</t>
   </si>
 </sst>
 </file>
@@ -445,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32442E77-81F3-40C4-8680-03E66F3A70A4}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,32 +464,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -503,43 +497,29 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
         <v>1</v>
       </c>
     </row>

</xml_diff>